<commit_message>
fix prefix range issue
</commit_message>
<xml_diff>
--- a/data/city/cn.v1.xlsx
+++ b/data/city/cn.v1.xlsx
@@ -3,13 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524C5762-5B8D-184A-862C-1A2A17C45EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC13AA3-8B00-7F4A-8817-FE3D66201315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="city" sheetId="1" r:id="rId1"/>
-    <sheet name="other" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -4921,7 +4920,7 @@
   <dimension ref="A1:CW373"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -13752,19 +13751,4 @@
     <ignoredError sqref="D2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373DC81F-5E87-A646-94C1-CBED2808CACF}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>